<commit_message>
Uploaded 03-九月-2019 14:07:49 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87E7B27-ABDF-8945-AF81-E541B3A3224E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7183B405-3AAA-E642-BBF2-6DBF8E390994}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37520" yWindow="480" windowWidth="37540" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
+    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="2" r:id="rId1"/>
@@ -104,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$policy.setName("$param")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陳小亮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,11 +124,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$policy.setAmount($param)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$policy.setName("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$policy.setAmount($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -295,37 +295,37 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +644,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -661,7 +661,7 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="16">
       <c r="A2" s="3" t="s">
@@ -670,110 +670,110 @@
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="16">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="16">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="34">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="34">
-      <c r="A9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="D10" s="7">
+        <v>600</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7">
         <v>600</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16">
-      <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="9">
-        <v>600</v>
-      </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Uploaded 03-九月-2019 14:09:58 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7183B405-3AAA-E642-BBF2-6DBF8E390994}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392CF74-4A09-A249-8B97-77D33AB9B8CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -207,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -278,13 +278,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -325,6 +362,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,7 +690,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -708,11 +754,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5">
@@ -776,9 +822,10 @@
       <c r="E11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded 03-九月-2019 14:12:42 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392CF74-4A09-A249-8B97-77D33AB9B8CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BD898B-E72C-FD42-8840-4ABA06DCCB79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -92,14 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$policy: Policy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$policy.setId("$param")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,11 +120,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$policy.setName("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$policy.setAmount($param);</t>
+    <t>Policy policy = new Policy();
+policy.setId("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>policy.setName("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>policy.setAmount($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -321,7 +318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -372,6 +369,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,7 +690,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -754,23 +754,21 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7"/>
-      <c r="B7" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="B7" s="16"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="48">
       <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
+      <c r="B8" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -782,10 +780,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -794,16 +792,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7">
         <v>600</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16">
@@ -811,10 +809,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="7">
         <v>600</v>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:35:20 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BD898B-E72C-FD42-8840-4ABA06DCCB79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8FEFDD-E8A9-2449-9C5F-3D8DB99F0132}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>RuleSet</t>
   </si>
@@ -132,12 +132,23 @@
     <t>policy.setAmount($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>$insured: Insured</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insuredId = $param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +187,12 @@
       <name val="PMingLiU"/>
       <family val="1"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -318,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -345,33 +362,37 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,60 +708,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A985E6-551A-B649-A4C9-6A30BB11FEB0}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="16">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="16">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="5" spans="1:5" ht="16">
+      <c r="C3" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="16">
       <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" ht="16">
+      <c r="B5" s="18"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>4</v>
+      <c r="B6" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -748,31 +771,40 @@
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="7"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="48">
+      <c r="B7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="48">
       <c r="A8" s="7"/>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="34">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="34">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -780,50 +812,59 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>600</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>600</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A5:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:37:38 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8FEFDD-E8A9-2449-9C5F-3D8DB99F0132}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD7207C-3D7F-7F40-8C50-CA780EB26C4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insuredId = $param</t>
+    <t>insuredId = "$param"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:38:57 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD7207C-3D7F-7F40-8C50-CA780EB26C4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098B05E-6AAB-EA44-B94E-B2BB840B436E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.redhat.prudential_poc.pojo.Policy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,6 +137,10 @@
   </si>
   <si>
     <t>insuredId = "$param"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.pojo.Insured,com.redhat.prudential_poc.pojo.Policy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -711,7 +711,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -781,7 +781,7 @@
     <row r="7" spans="1:6">
       <c r="A7" s="7"/>
       <c r="B7" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -791,16 +791,16 @@
     <row r="8" spans="1:6" ht="48">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="7"/>
     </row>
@@ -815,10 +815,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7"/>
     </row>
@@ -827,19 +827,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="7">
         <v>600</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16">
@@ -847,13 +847,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="7">
         <v>600</v>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:40:25 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098B05E-6AAB-EA44-B94E-B2BB840B436E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC54678A-100D-DE4D-B3AD-62BBF6ADF7D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>RuleSet</t>
   </si>
@@ -136,11 +136,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insuredId = "$param"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>com.redhat.prudential_poc.pojo.Insured,com.redhat.prudential_poc.pojo.Policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insuredId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A223456789"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A223456123"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -711,7 +719,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -736,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -791,7 +799,7 @@
     <row r="8" spans="1:6" ht="48">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>20</v>
@@ -827,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>15</v>
@@ -847,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 22:31:41 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC54678A-100D-DE4D-B3AD-62BBF6ADF7D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8267CD-CBDE-EF45-BAD3-E0824B89F638}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -116,19 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Policy policy = new Policy();
-policy.setId("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>policy.setName("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>policy.setAmount($param);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CONDITION</t>
   </si>
   <si>
@@ -149,6 +136,19 @@
   </si>
   <si>
     <t>"A223456123"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Policy $policy = new Policy();
+$policy.setId("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$policy.setName("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$policy.setAmount($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,26 +379,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -719,7 +719,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -744,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -758,10 +758,10 @@
       <c r="C3" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="16">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -770,8 +770,8 @@
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>23</v>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -788,27 +788,27 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7"/>
-      <c r="B7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="48">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7"/>
     </row>
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>15</v>
@@ -846,7 +846,7 @@
       <c r="E10" s="7">
         <v>600</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -855,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>16</v>
@@ -866,7 +866,7 @@
       <c r="E11" s="7">
         <v>600</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 22:42:35 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8267CD-CBDE-EF45-BAD3-E0824B89F638}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66650D19-D47A-084C-8308-8C7C414FFE94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -139,16 +139,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Policy $policy = new Policy();
+    <t>$policy.setName("$param");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$policy.setAmount($param);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System.out.println("=== Fire policy!!! ===");
+Policy $policy = new Policy();
 $policy.setId("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$policy.setName("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$policy.setAmount($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -719,7 +720,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -796,19 +797,19 @@
       <c r="E7" s="18"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="48">
+    <row r="8" spans="1:6" ht="80">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="7"/>
     </row>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 23:14:05 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66650D19-D47A-084C-8308-8C7C414FFE94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06C5853-B88A-B347-968E-495635D65D26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -88,26 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陳小亮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A223456789</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A223456123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陳老爺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>保單總額</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,10 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.redhat.prudential_poc.pojo.Insured,com.redhat.prudential_poc.pojo.Policy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insuredId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,17 +115,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$policy.setName("$param");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$policy.setAmount($param);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System.out.println("=== Fire policy!!! ===");
-Policy $policy = new Policy();
-$policy.setId("$param");</t>
+    <t>com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$insured.setTotoalAmt($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -230,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -316,17 +286,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -344,7 +303,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -377,25 +336,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -717,163 +667,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A985E6-551A-B649-A4C9-6A30BB11FEB0}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="16">
+    </row>
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="5" spans="1:6" ht="16">
-      <c r="A5" s="19" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" ht="16">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>20</v>
+      <c r="B6" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:4">
       <c r="A7" s="7"/>
-      <c r="B7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="80">
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="34">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="34">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="16">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7">
+        <v>600</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7">
-        <v>600</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16">
+    </row>
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="7">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7">
         <v>600</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="D11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A5:E5"/>
+  <mergeCells count="2">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 23:15:04 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06C5853-B88A-B347-968E-495635D65D26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3581E115-60E3-8142-85F3-E5DDCA903972}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$insured.setTotoalAmt($param);</t>
+    <t>$insured.getTotalAmt($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 23:15:42 {/src/main/resources/com/redhat/prudential_poc/Policy.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3581E115-60E3-8142-85F3-E5DDCA903972}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF050C4-58B6-C043-A99E-ECDA8E89CAFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$insured.getTotalAmt($param);</t>
+    <t>$insured.setTotalAmt($param);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,7 +670,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>